<commit_message>
Added Onsale promotion, print recipt functionality and other changes.
</commit_message>
<xml_diff>
--- a/GroceryCoCheckout/Data/Catalog.xlsx
+++ b/GroceryCoCheckout/Data/Catalog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Name</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t>Bananas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Promotions </t>
   </si>
 </sst>
 </file>
@@ -403,9 +400,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -415,9 +410,6 @@
       <c r="B2">
         <v>1.99</v>
       </c>
-      <c r="C2">
-        <v>50</v>
-      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -426,9 +418,6 @@
       <c r="B3">
         <v>4.5999999999999996</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -436,9 +425,6 @@
       </c>
       <c r="B4">
         <v>0.99</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Group price promotion
</commit_message>
<xml_diff>
--- a/GroceryCoCheckout/Data/Catalog.xlsx
+++ b/GroceryCoCheckout/Data/Catalog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Name</t>
   </si>
@@ -29,6 +29,12 @@
   </si>
   <si>
     <t>Bananas</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>Tomato</t>
   </si>
 </sst>
 </file>
@@ -379,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -427,6 +433,22 @@
         <v>0.99</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>